<commit_message>
perbaikan perhitungan c45 ke 5
</commit_message>
<xml_diff>
--- a/asset/data_testing1.xlsx
+++ b/asset/data_testing1.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="192">
   <si>
     <t>NAMA</t>
   </si>
@@ -628,37 +628,25 @@
     <t>2.4 IPS2 KURANG THEN TERLAMBAT</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>npm</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>jk</t>
-  </si>
-  <si>
-    <t>ips1</t>
-  </si>
-  <si>
-    <t>ips2</t>
-  </si>
-  <si>
-    <t>ips3</t>
-  </si>
-  <si>
-    <t>ips4</t>
-  </si>
-  <si>
     <t>REZHA</t>
   </si>
   <si>
-    <t>VIKRI</t>
-  </si>
-  <si>
-    <t>SEPTI</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>JAKA</t>
+  </si>
+  <si>
+    <t>JOKO</t>
+  </si>
+  <si>
+    <t>JAMOL</t>
+  </si>
+  <si>
+    <t>SASA</t>
+  </si>
+  <si>
+    <t>SOLI</t>
   </si>
 </sst>
 </file>
@@ -671,7 +659,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;???_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +736,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -770,12 +766,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -798,12 +793,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -844,19 +855,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -891,7 +900,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C4FF36-8148-0784-02D0-C24DAB88A520}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6C4FF36-8148-0784-02D0-C24DAB88A520}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1229,7 +1238,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12532,160 +12541,296 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.375" style="30" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
     <col min="4" max="4" width="15.625" customWidth="1"/>
     <col min="5" max="5" width="16.375" customWidth="1"/>
     <col min="6" max="6" width="20.125" customWidth="1"/>
     <col min="7" max="7" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:9" ht="15">
+      <c r="A1" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32">
+        <v>2020804139</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="D2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2020804179</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D3" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
+      <c r="A4" s="32">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32">
+        <v>2020434179</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32">
+        <v>2020434179</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15">
+      <c r="A6" s="32">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32">
+        <v>2020804139</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="32">
+        <v>6</v>
+      </c>
+      <c r="B7" s="32">
+        <v>2020804179</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="A8" s="32">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32">
+        <v>2020434179</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="D8" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="32">
+        <v>8</v>
+      </c>
+      <c r="B9" s="32">
+        <v>2020434179</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2020804139</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="34" t="s">
+      <c r="D9" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="34">
-        <v>3.7</v>
-      </c>
-      <c r="F2" s="34">
-        <v>3.2</v>
-      </c>
-      <c r="G2" s="34">
-        <v>2.8</v>
-      </c>
-      <c r="H2" s="34">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2020804149</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="F3" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="G3" s="34">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H3" s="34">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2020804134</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="34">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F4" s="34">
-        <v>3.6</v>
-      </c>
-      <c r="G4" s="34">
-        <v>3.5</v>
-      </c>
-      <c r="H4" s="34">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="E9" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:8">
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="B16"/>
     </row>
     <row r="17" spans="2:2">
@@ -12720,6 +12865,48 @@
     </row>
     <row r="27" spans="2:2">
       <c r="B27"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41"/>
     </row>
     <row r="46" spans="2:2" ht="15.75">
       <c r="B46" s="29"/>

</xml_diff>